<commit_message>
Added changes, splitted tests: unic for each data set
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Монумент Астана-Байтерек</t>
   </si>
@@ -34,42 +34,31 @@
     <t xml:space="preserve">59.9992052, 30.2891141</t>
   </si>
   <si>
-    <t xml:space="preserve">Дворцовая площадь,  Санкт-Петербург</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59.93909545, 30.3156973654466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Набережные Челны</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55.7420117, 52.3992173</t>
-  </si>
-  <si>
     <t xml:space="preserve">212 Baker St, Marylebone, London</t>
   </si>
   <si>
     <t xml:space="preserve">51.5242146, -0.1584717</t>
   </si>
   <si>
-    <t xml:space="preserve">Пекин</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39.906217, 116.3912757</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Παρθενώνας</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.9715141, 23.7266498463072</t>
+    <t xml:space="preserve">jhbkvcz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ыпчваспрмглш</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -136,13 +125,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -165,14 +158,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,32 +195,26 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>1234132456549</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.8765432</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>